<commit_message>
final edits to thesis
</commit_message>
<xml_diff>
--- a/TradingThesis/figures/momentumdata.xlsx
+++ b/TradingThesis/figures/momentumdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlexT/Dropbox/SEN19R/FIRST/algorithmic-trading/TradingThesis/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC75F1AE-B377-6D4B-B39F-3804DAEE19C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF044093-855C-9741-BCB2-256FBC2BB5AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="740" windowWidth="25500" windowHeight="15100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="740" windowWidth="25860" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,23 +42,7 @@
     <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$13:$D$27</definedName>
     <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$F$12</definedName>
     <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$F$13:$F$27</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$C$12</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$C$13:$C$27</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$D$12</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$D$13:$D$27</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$E$12</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$E$13:$E$27</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$F$12</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$F$13:$F$27</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$E$12</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$C$12</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$C$13:$C$27</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$D$12</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$D$13:$D$27</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$E$12</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$E$13:$E$27</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$F$12</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$F$13:$F$27</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$E$13:$E$27</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$F$12</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$F$13:$F$27</definedName>
@@ -730,62 +714,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>Momentum Strategies Return</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1156,7 +1085,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="137"/>
         <c:overlap val="-27"/>
         <c:axId val="1722815839"/>
         <c:axId val="1723039487"/>
@@ -1190,12 +1119,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1240,12 +1166,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1254,13 +1177,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Percentage Profit Difference</a:t>
+                  <a:t> Difference between strategy and baseline (%)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> between Strategy and Baseline (%)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1277,12 +1195,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1309,12 +1224,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1351,12 +1263,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1391,7 +1300,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1400">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1409,60 +1322,32 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.17</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.19</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.23</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0">
-      <cx:tx>
-        <cx:txData>
-          <cx:v>Momentum Strategies Total Performance</cx:v>
-        </cx:txData>
-      </cx:tx>
-      <cx:txPr>
-        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr" rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Momentum Strategies Total Performance</a:t>
-          </a:r>
-        </a:p>
-      </cx:txPr>
-    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="boxWhisker" uniqueId="{6B87F321-4A1E-1A44-9F1B-287B64FC9E8C}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.16</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>SMA </cx:v>
             </cx:txData>
           </cx:tx>
@@ -1475,7 +1360,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{AF38F9C0-230A-D746-B4E7-35FEDFE847BE}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.18</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>EMA </cx:v>
             </cx:txData>
           </cx:tx>
@@ -1488,7 +1373,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{5E460381-89FA-884B-9B6F-B342BFAAD0AF}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.20</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>Bollinger Bands </cx:v>
             </cx:txData>
           </cx:tx>
@@ -1501,7 +1386,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{9D90C959-4D17-A842-B7C3-13A71A069895}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.22</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>RSI </cx:v>
             </cx:txData>
           </cx:tx>
@@ -1513,8 +1398,29 @@
         </cx:series>
       </cx:plotAreaRegion>
       <cx:axis id="0" hidden="1">
-        <cx:catScaling gapWidth="1.5"/>
+        <cx:catScaling gapWidth="0.100000001"/>
         <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1300" b="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1300">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling max="300" min="-310"/>
@@ -1539,29 +1445,27 @@
                   <a:buFontTx/>
                   <a:buNone/>
                   <a:tabLst/>
-                  <a:defRPr/>
+                  <a:defRPr sz="1300">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:rPr lang="en-US" sz="1300" b="0" i="0" u="none" strike="noStrike" baseline="0">
                     <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:sysClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:effectLst/>
                     <a:latin typeface="Calibri"/>
                     <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>Percentage difference in profit from baseline (%)</a:t>
+                  <a:t>Difference in profit from baseline (%)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:endParaRPr lang="en-US" sz="1300" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:sysClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Calibri"/>
                 </a:endParaRPr>
@@ -1572,9 +1476,48 @@
         <cx:majorGridlines/>
         <cx:majorTickMarks type="out"/>
         <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1300">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1300" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
       </cx:axis>
     </cx:plotArea>
-    <cx:legend pos="r" align="ctr" overlay="0"/>
+    <cx:legend pos="r" align="ctr" overlay="0">
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1300">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1300" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+      </cx:txPr>
+    </cx:legend>
   </cx:chart>
 </cx:chartSpace>
 </file>
@@ -2753,16 +2696,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>139699</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>84996</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>706966</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>88899</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -2798,8 +2741,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5435599" y="1473200"/>
-              <a:ext cx="9482667" cy="5689600"/>
+              <a:off x="14350999" y="1100996"/>
+              <a:ext cx="5003801" cy="4474303"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3156,8 +3099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>